<commit_message>
Graphs and some adjustments to the previous sections
</commit_message>
<xml_diff>
--- a/Data/births.xlsx
+++ b/Data/births.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzelegesari/Documents/GitHub/emu660-spring2025-Selenzel/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A8380A-3F33-1347-B93C-70382F108B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4729717D-0319-7342-B8D1-64BDFA2DB619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="2320" windowWidth="25840" windowHeight="14240" xr2:uid="{37EC6BE8-07D9-3547-B734-125D0061910C}"/>
+    <workbookView xWindow="2680" yWindow="2180" windowWidth="25840" windowHeight="14240" xr2:uid="{37EC6BE8-07D9-3547-B734-125D0061910C}"/>
   </bookViews>
   <sheets>
     <sheet name="Doğum" sheetId="1" r:id="rId1"/>
@@ -296,10 +296,10 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Gender _Baby</t>
+    <t>Births</t>
   </si>
   <si>
-    <t>Births</t>
+    <t>Gender_Baby</t>
   </si>
 </sst>
 </file>
@@ -704,13 +704,13 @@
         <v>83</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>